<commit_message>
Updates to supervision forms
</commit_message>
<xml_diff>
--- a/app/config/tables/SUPERVISIONTAB/Forms/SUPERVISIONTAB/SUPERVISIONTAB.xlsx
+++ b/app/config/tables/SUPERVISIONTAB/Forms/SUPERVISIONTAB/SUPERVISIONTAB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41C1606-570C-49E1-A208-6A0CA3DFBB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5997C31A-C612-4DC2-B501-04BEE4376786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="286">
   <si>
     <t>setting_name</t>
   </si>
@@ -267,12 +267,6 @@
     <t>Julie</t>
   </si>
   <si>
-    <t>SOT</t>
-  </si>
-  <si>
-    <t>Name of SOT</t>
-  </si>
-  <si>
     <t>select_one</t>
   </si>
   <si>
@@ -384,9 +378,6 @@
     <t>Tablet charger</t>
   </si>
   <si>
-    <t>Clipboard</t>
-  </si>
-  <si>
     <t>MUAC</t>
   </si>
   <si>
@@ -438,12 +429,6 @@
     <t>Saldo</t>
   </si>
   <si>
-    <t>Inernet box</t>
-  </si>
-  <si>
-    <t>Caixa de internet</t>
-  </si>
-  <si>
     <t>MaterialGiven</t>
   </si>
   <si>
@@ -666,9 +651,6 @@
     <t xml:space="preserve">Other relevant observations? Anything the investigators and/or other supervisors should know? </t>
   </si>
   <si>
-    <t>Nome de SOT</t>
-  </si>
-  <si>
     <t xml:space="preserve">ASC presente? </t>
   </si>
   <si>
@@ -880,6 +862,36 @@
   </si>
   <si>
     <t>Você está prestes a supervisionar em:</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>Does the SOT need more supervision to be able to register pregnancies without help</t>
+  </si>
+  <si>
+    <t>Does the SOT need more supervision to be able to conduct follow-up without help?</t>
+  </si>
+  <si>
+    <t>O SOT precisa de mais supervisão para poder registrar gravidezes sem ajuda</t>
+  </si>
+  <si>
+    <t>O SOT precisa de mais supervisão para poder fazer o seguimento sem ajuda?</t>
+  </si>
+  <si>
+    <t>MORESUPREG</t>
+  </si>
+  <si>
+    <t>MORESUPFU</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Internet box</t>
+  </si>
+  <si>
+    <t>Box de internet</t>
   </si>
 </sst>
 </file>
@@ -1412,8 +1424,8 @@
   <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,32 +1578,30 @@
     </row>
     <row r="12" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="B12" s="11" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="11" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>276</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1602,32 +1612,30 @@
     </row>
     <row r="15" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="11" t="str">
-        <f>"1"</f>
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="11" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
       <c r="C16" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1638,450 +1646,450 @@
     </row>
     <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="D21" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="D33" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>284</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
+        <v>284</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="D45" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D48" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D50" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D51" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2090,7 +2098,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B53" t="str">
         <f>"1"</f>
@@ -2105,7 +2113,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B54" t="str">
         <f>"2"</f>
@@ -2120,17 +2128,17 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B55" s="12" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2771,11 +2779,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:T106"/>
+  <dimension ref="A1:T109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2872,57 +2880,57 @@
     </row>
     <row r="3" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="H3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="R3" s="10"/>
     </row>
     <row r="4" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="R4" s="10"/>
     </row>
     <row r="5" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="R5" s="10"/>
     </row>
     <row r="6" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -2934,13 +2942,13 @@
         <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="G7" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H7" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2948,13 +2956,16 @@
         <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="H8" t="s">
-        <v>269</v>
+        <v>263</v>
+      </c>
+      <c r="P8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2969,88 +2980,91 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>44</v>
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>252</v>
       </c>
       <c r="G11" t="s">
         <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="B12" t="s">
         <v>79</v>
       </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>258</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="C12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>80</v>
       </c>
-      <c r="H12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" t="s">
-        <v>212</v>
-      </c>
+      <c r="R14" s="19"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>82</v>
-      </c>
-      <c r="R15" s="19"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>36</v>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -3058,657 +3072,654 @@
         <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
         <v>99</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>100</v>
       </c>
-      <c r="H20" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>257</v>
+      <c r="H21" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" t="s">
-        <v>216</v>
+      <c r="B22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>36</v>
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" t="s">
+        <v>213</v>
+      </c>
+      <c r="G25" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" t="s">
+        <v>214</v>
+      </c>
+      <c r="G26" t="s">
         <v>103</v>
       </c>
-      <c r="F26" t="s">
-        <v>219</v>
-      </c>
-      <c r="G26" t="s">
-        <v>104</v>
-      </c>
       <c r="H26" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" t="s">
-        <v>220</v>
-      </c>
-      <c r="G27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" t="s">
-        <v>217</v>
+      <c r="B27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" t="s">
-        <v>108</v>
-      </c>
-      <c r="G30" t="s">
-        <v>109</v>
-      </c>
-      <c r="H30" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" t="s">
+        <v>110</v>
+      </c>
+      <c r="H32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" t="s">
-        <v>111</v>
-      </c>
-      <c r="G33" t="s">
-        <v>112</v>
-      </c>
-      <c r="H33" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" t="s">
+        <v>132</v>
+      </c>
+      <c r="G35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" t="s">
-        <v>136</v>
-      </c>
-      <c r="F36" t="s">
-        <v>137</v>
-      </c>
-      <c r="G36" t="s">
-        <v>138</v>
-      </c>
-      <c r="H36" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>36</v>
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" t="s">
+        <v>139</v>
+      </c>
+      <c r="H38" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+      <c r="B39" t="s">
         <v>79</v>
       </c>
-      <c r="E39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="C39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" t="s">
         <v>143</v>
       </c>
-      <c r="G39" t="s">
-        <v>144</v>
-      </c>
-      <c r="H39" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" t="s">
-        <v>145</v>
+      <c r="H40" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>146</v>
+        <v>77</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
       </c>
       <c r="F41" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" t="s">
         <v>147</v>
       </c>
-      <c r="G41" t="s">
-        <v>148</v>
-      </c>
       <c r="H41" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E42" t="s">
         <v>46</v>
       </c>
       <c r="F42" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H42" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s">
         <v>46</v>
       </c>
       <c r="F43" t="s">
+        <v>146</v>
+      </c>
+      <c r="G43" t="s">
+        <v>149</v>
+      </c>
+      <c r="H43" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>150</v>
-      </c>
-      <c r="G43" t="s">
-        <v>153</v>
-      </c>
-      <c r="H43" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" t="s">
-        <v>46</v>
-      </c>
-      <c r="F44" t="s">
-        <v>151</v>
-      </c>
-      <c r="G44" t="s">
-        <v>154</v>
-      </c>
-      <c r="H44" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>36</v>
+      <c r="D47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" t="s">
+        <v>152</v>
+      </c>
+      <c r="G47" t="s">
+        <v>153</v>
+      </c>
+      <c r="H47" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+      <c r="B48" t="s">
         <v>79</v>
       </c>
-      <c r="E48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" t="s">
-        <v>157</v>
-      </c>
-      <c r="G48" t="s">
-        <v>158</v>
-      </c>
-      <c r="H48" t="s">
-        <v>237</v>
+      <c r="C48" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" t="s">
-        <v>156</v>
+      <c r="D49" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" t="s">
+        <v>154</v>
+      </c>
+      <c r="G49" t="s">
+        <v>143</v>
+      </c>
+      <c r="H49" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>146</v>
+        <v>77</v>
+      </c>
+      <c r="E50" t="s">
+        <v>156</v>
       </c>
       <c r="F50" t="s">
         <v>159</v>
       </c>
       <c r="G50" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E51" t="s">
+        <v>156</v>
+      </c>
+      <c r="F51" t="s">
+        <v>160</v>
+      </c>
+      <c r="G51" t="s">
         <v>161</v>
       </c>
-      <c r="F51" t="s">
-        <v>164</v>
-      </c>
-      <c r="G51" t="s">
-        <v>160</v>
-      </c>
       <c r="H51" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>79</v>
-      </c>
-      <c r="E52" t="s">
-        <v>161</v>
-      </c>
-      <c r="F52" t="s">
-        <v>165</v>
-      </c>
-      <c r="G52" t="s">
-        <v>166</v>
-      </c>
-      <c r="H52" t="s">
-        <v>239</v>
+      <c r="B52" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>36</v>
+      <c r="D55" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55" t="s">
+        <v>163</v>
+      </c>
+      <c r="G55" t="s">
+        <v>162</v>
+      </c>
+      <c r="H55" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+      <c r="B56" t="s">
         <v>79</v>
       </c>
-      <c r="E56" t="s">
-        <v>46</v>
-      </c>
-      <c r="F56" t="s">
-        <v>168</v>
-      </c>
-      <c r="G56" t="s">
-        <v>167</v>
-      </c>
-      <c r="H56" t="s">
-        <v>240</v>
+      <c r="C56" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" t="s">
-        <v>171</v>
+      <c r="D57" t="s">
+        <v>141</v>
+      </c>
+      <c r="F57" t="s">
+        <v>164</v>
+      </c>
+      <c r="G57" t="s">
+        <v>143</v>
+      </c>
+      <c r="H57" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>146</v>
+        <v>77</v>
+      </c>
+      <c r="E58" t="s">
+        <v>46</v>
       </c>
       <c r="F58" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G58" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="H58" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E59" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="F59" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G59" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H59" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>79</v>
-      </c>
-      <c r="E60" t="s">
-        <v>161</v>
-      </c>
-      <c r="F60" t="s">
-        <v>174</v>
-      </c>
-      <c r="G60" t="s">
-        <v>173</v>
-      </c>
-      <c r="H60" t="s">
-        <v>242</v>
+      <c r="B60" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>37</v>
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" t="s">
-        <v>171</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>36</v>
+      <c r="D64" t="s">
+        <v>77</v>
+      </c>
+      <c r="E64" t="s">
+        <v>156</v>
+      </c>
+      <c r="F64" t="s">
+        <v>170</v>
+      </c>
+      <c r="G64" t="s">
+        <v>177</v>
+      </c>
+      <c r="H64" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E65" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F65" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G65" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H65" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E66" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F66" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G66" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H66" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E67" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F67" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G67" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H67" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>79</v>
-      </c>
-      <c r="E68" t="s">
-        <v>161</v>
-      </c>
-      <c r="F68" t="s">
-        <v>178</v>
-      </c>
-      <c r="G68" t="s">
-        <v>179</v>
-      </c>
-      <c r="H68" t="s">
-        <v>246</v>
+      <c r="B68" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>36</v>
+      <c r="D71" t="s">
+        <v>77</v>
+      </c>
+      <c r="E71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" t="s">
+        <v>178</v>
+      </c>
+      <c r="G71" t="s">
+        <v>179</v>
+      </c>
+      <c r="H71" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+      <c r="B72" t="s">
         <v>79</v>
       </c>
-      <c r="E72" t="s">
-        <v>46</v>
-      </c>
-      <c r="F72" t="s">
-        <v>183</v>
-      </c>
-      <c r="G72" t="s">
-        <v>184</v>
-      </c>
-      <c r="H72" t="s">
-        <v>247</v>
+      <c r="C72" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>81</v>
-      </c>
-      <c r="C73" t="s">
-        <v>185</v>
+      <c r="D73" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" t="s">
+        <v>181</v>
+      </c>
+      <c r="G73" t="s">
+        <v>182</v>
+      </c>
+      <c r="H73" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>44</v>
+        <v>77</v>
+      </c>
+      <c r="E74" t="s">
+        <v>46</v>
       </c>
       <c r="F74" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G74" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H74" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>79</v>
-      </c>
-      <c r="E75" t="s">
-        <v>46</v>
-      </c>
-      <c r="F75" t="s">
-        <v>188</v>
-      </c>
-      <c r="G75" t="s">
-        <v>189</v>
-      </c>
-      <c r="H75" t="s">
-        <v>249</v>
+      <c r="B75" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>36</v>
+      <c r="D78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E78" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" t="s">
+        <v>185</v>
+      </c>
+      <c r="G78" t="s">
+        <v>189</v>
+      </c>
+      <c r="H78" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
+      <c r="B79" t="s">
         <v>79</v>
       </c>
-      <c r="E79" t="s">
-        <v>46</v>
-      </c>
-      <c r="F79" t="s">
-        <v>190</v>
-      </c>
-      <c r="G79" t="s">
-        <v>194</v>
-      </c>
-      <c r="H79" t="s">
-        <v>250</v>
+      <c r="C79" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" t="s">
-        <v>193</v>
+      <c r="D80" t="s">
+        <v>44</v>
+      </c>
+      <c r="F80" t="s">
+        <v>186</v>
+      </c>
+      <c r="G80" t="s">
+        <v>182</v>
+      </c>
+      <c r="H80" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
@@ -3716,257 +3727,287 @@
         <v>44</v>
       </c>
       <c r="F81" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G81" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H81" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
-        <v>44</v>
-      </c>
-      <c r="F82" t="s">
-        <v>192</v>
-      </c>
-      <c r="G82" t="s">
-        <v>195</v>
-      </c>
-      <c r="H82" t="s">
-        <v>251</v>
+      <c r="B82" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>36</v>
+      <c r="D85" t="s">
+        <v>77</v>
+      </c>
+      <c r="E85" t="s">
+        <v>46</v>
+      </c>
+      <c r="F85" t="s">
+        <v>191</v>
+      </c>
+      <c r="G85" t="s">
+        <v>192</v>
+      </c>
+      <c r="H85" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
+      <c r="B86" t="s">
         <v>79</v>
       </c>
-      <c r="E86" t="s">
-        <v>46</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="C86" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>44</v>
+      </c>
+      <c r="F87" t="s">
         <v>196</v>
       </c>
-      <c r="G86" t="s">
-        <v>197</v>
-      </c>
-      <c r="H86" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>81</v>
-      </c>
-      <c r="C87" t="s">
-        <v>200</v>
+      <c r="G87" t="s">
+        <v>193</v>
+      </c>
+      <c r="H87" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>44</v>
+        <v>77</v>
+      </c>
+      <c r="E88" t="s">
+        <v>46</v>
       </c>
       <c r="F88" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G88" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H88" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
-        <v>79</v>
-      </c>
-      <c r="E89" t="s">
-        <v>46</v>
-      </c>
-      <c r="F89" t="s">
-        <v>202</v>
-      </c>
-      <c r="G89" t="s">
-        <v>199</v>
-      </c>
-      <c r="H89" t="s">
-        <v>254</v>
+      <c r="B89" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>36</v>
+      <c r="D92" t="s">
+        <v>77</v>
+      </c>
+      <c r="E92" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" t="s">
+        <v>198</v>
+      </c>
+      <c r="G92" t="s">
+        <v>199</v>
+      </c>
+      <c r="H92" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
+      <c r="B93" t="s">
         <v>79</v>
       </c>
-      <c r="E93" t="s">
+      <c r="C93" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>44</v>
+      </c>
+      <c r="F94" t="s">
+        <v>201</v>
+      </c>
+      <c r="G94" t="s">
+        <v>202</v>
+      </c>
+      <c r="H94" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>77</v>
+      </c>
+      <c r="E96" t="s">
         <v>46</v>
       </c>
-      <c r="F93" t="s">
-        <v>203</v>
-      </c>
-      <c r="G93" t="s">
-        <v>204</v>
-      </c>
-      <c r="H93" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>81</v>
-      </c>
-      <c r="C94" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D95" t="s">
+      <c r="F96" t="s">
+        <v>134</v>
+      </c>
+      <c r="G96" t="s">
+        <v>135</v>
+      </c>
+      <c r="H96" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>79</v>
+      </c>
+      <c r="C97" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
         <v>44</v>
       </c>
-      <c r="F95" t="s">
-        <v>206</v>
-      </c>
-      <c r="G95" t="s">
-        <v>207</v>
-      </c>
-      <c r="H95" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+      <c r="F98" t="s">
+        <v>137</v>
+      </c>
+      <c r="G98" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D97" t="s">
-        <v>44</v>
-      </c>
-      <c r="F97" t="s">
-        <v>208</v>
-      </c>
-      <c r="G97" t="s">
-        <v>209</v>
-      </c>
-      <c r="H97" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>37</v>
+      <c r="H98" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D100" t="s">
-        <v>79</v>
-      </c>
-      <c r="E100" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F100" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="G100" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="H100" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>81</v>
-      </c>
-      <c r="C101" t="s">
-        <v>141</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D102" t="s">
-        <v>44</v>
-      </c>
-      <c r="F102" t="s">
-        <v>142</v>
-      </c>
-      <c r="G102" t="s">
-        <v>84</v>
-      </c>
-      <c r="H102" t="s">
-        <v>231</v>
+      <c r="B102" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>82</v>
+      <c r="D103" t="s">
+        <v>77</v>
+      </c>
+      <c r="E103" t="s">
+        <v>156</v>
+      </c>
+      <c r="F103" t="s">
+        <v>281</v>
+      </c>
+      <c r="G103" t="s">
+        <v>277</v>
+      </c>
+      <c r="H103" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
-        <v>103</v>
+        <v>77</v>
+      </c>
+      <c r="E104" t="s">
+        <v>156</v>
       </c>
       <c r="F104" t="s">
-        <v>221</v>
+        <v>282</v>
       </c>
       <c r="G104" t="s">
-        <v>224</v>
+        <v>278</v>
       </c>
       <c r="H104" t="s">
-        <v>225</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
-        <v>103</v>
-      </c>
-      <c r="F105" t="s">
-        <v>222</v>
-      </c>
-      <c r="G105" t="s">
-        <v>223</v>
-      </c>
-      <c r="H105" t="s">
-        <v>226</v>
+      <c r="B105" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>101</v>
+      </c>
+      <c r="F107" t="s">
+        <v>215</v>
+      </c>
+      <c r="G107" t="s">
+        <v>218</v>
+      </c>
+      <c r="H107" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>101</v>
+      </c>
+      <c r="F108" t="s">
+        <v>216</v>
+      </c>
+      <c r="G108" t="s">
+        <v>217</v>
+      </c>
+      <c r="H108" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4070,11 +4111,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4102,10 +4143,10 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -4113,7 +4154,7 @@
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
@@ -4124,10 +4165,10 @@
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -4135,7 +4176,7 @@
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -4146,10 +4187,10 @@
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -4157,7 +4198,7 @@
     </row>
     <row r="7" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>44</v>
@@ -4168,7 +4209,7 @@
     </row>
     <row r="8" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -4180,7 +4221,7 @@
     <row r="9" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B10" t="s">
         <v>69</v>
@@ -4194,10 +4235,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" t="s">
         <v>77</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -4208,10 +4249,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -4225,31 +4266,29 @@
         <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
-      <c r="G13"/>
       <c r="H13"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
       </c>
-      <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
         <v>69</v>
@@ -4264,53 +4303,54 @@
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" t="s">
         <v>101</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" t="b">
         <v>0</v>
       </c>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -4318,145 +4358,144 @@
       <c r="E20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
-      <c r="E21"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
       </c>
       <c r="E23"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>146</v>
       </c>
-      <c r="C24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24"/>
-      <c r="G24"/>
-    </row>
-    <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>150</v>
-      </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
       </c>
-      <c r="G26"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>159</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>164</v>
       </c>
-      <c r="B30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G30"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>165</v>
-      </c>
-      <c r="B31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" t="b">
-        <v>0</v>
-      </c>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>168</v>
-      </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -4465,10 +4504,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -4477,10 +4516,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -4489,22 +4528,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
-      <c r="G35"/>
+      <c r="E35"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -4513,10 +4552,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -4525,10 +4564,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -4540,19 +4579,18 @@
         <v>178</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
       </c>
-      <c r="E39"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -4560,10 +4598,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -4571,21 +4609,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
       </c>
+      <c r="E42"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -4594,7 +4633,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
@@ -4602,14 +4641,13 @@
       <c r="C44" t="b">
         <v>0</v>
       </c>
-      <c r="E44"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -4620,7 +4658,7 @@
         <v>196</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -4628,10 +4666,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -4639,29 +4677,29 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>203</v>
-      </c>
-      <c r="B49" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>206</v>
       </c>
       <c r="B50" t="s">
         <v>44</v>
@@ -4670,90 +4708,100 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>208</v>
+        <v>281</v>
       </c>
       <c r="B51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>282</v>
+      </c>
+      <c r="B52" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="s">
         <v>44</v>
       </c>
-      <c r="C51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>139</v>
-      </c>
-      <c r="B52" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>142</v>
-      </c>
-      <c r="B53" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>221</v>
-      </c>
-      <c r="B54" t="s">
-        <v>103</v>
-      </c>
       <c r="C54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>216</v>
+      </c>
+      <c r="B56" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+      <c r="B57"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C58"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+      <c r="B61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C64"/>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
@@ -4812,6 +4860,9 @@
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>